<commit_message>
import top tim excell
</commit_message>
<xml_diff>
--- a/public/assets/xls/toptim-import.xlsx
+++ b/public/assets/xls/toptim-import.xlsx
@@ -116,7 +116,7 @@
     <t>818_1_BENDAGGIO BLU.jpg, 818_244_BENDAGGIO TRICOLORE.jpg, 818_245_BENDAGGIO GRIGIO.jpg, 818_246_BENDAGGIO CAMO VERDE.jpg, 818_247_BENDAGGIO CAMO BLU.jpg, 818_24_BENDAGGIO ROSSO.jpg, 818_2_BENDAGGIO NERO.jpg, 818_96_BENDAGGIO GIALLO FLUO.jpg</t>
   </si>
   <si>
-    <t>100% pamuk</t>
+    <t>100% Pamuk</t>
   </si>
   <si>
     <t>crna.jpg, crvena.jpg, fluo žuta.jpg, maskirno plava.jpg, maskirno zelena.jpg, plava.jpg, siva.jpg, trobojnica.jpg, zelena.jpg, žuta.jpg</t>
@@ -158,7 +158,7 @@
     <t>820_2_unnamed.jpg</t>
   </si>
   <si>
-    <t>Umjetna koža</t>
+    <t>Umjetna Koža</t>
   </si>
   <si>
     <t>Rukavice Camouflage</t>
@@ -194,7 +194,7 @@
     <t>1049_2_guantoni senza dita MMA.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">"Izvana: UMJETNA KOŽA FLEX PU IZNUTRA: GUMENA </t>
+    <t>Izvana: Umjetna Koža Flex Pu Iznutra: Gumena Eva</t>
   </si>
   <si>
     <t>Rukavice Training</t>
@@ -212,7 +212,7 @@
     <t>819_24_GUANTONE TRAINING ROSSO.jpg, 819_26_GUANTONE TRAINING VERDE.jpg, 819_3_GUANTONE TRAINING ROYALL.jpg</t>
   </si>
   <si>
-    <t>Sintetička koža - koža</t>
+    <t>Sintetička Koža - Koža</t>
   </si>
   <si>
     <t>crvena.jpg, royal plava.jpg, zelena.jpg</t>
@@ -447,7 +447,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -478,15 +478,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -510,6 +513,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
@@ -1585,7 +1591,7 @@
     <col min="5" max="5" width="52" style="1" customWidth="1"/>
     <col min="6" max="6" width="27.5" style="1" customWidth="1"/>
     <col min="7" max="7" width="32.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="95.5391" style="1" customWidth="1"/>
+    <col min="8" max="8" width="30" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.1719" style="1" customWidth="1"/>
     <col min="10" max="10" width="7.85156" style="1" customWidth="1"/>
     <col min="11" max="11" width="7.17188" style="1" customWidth="1"/>
@@ -1742,7 +1748,7 @@
       <c r="E3" t="s" s="8">
         <v>33</v>
       </c>
-      <c r="F3" t="s" s="10">
+      <c r="F3" t="s" s="13">
         <v>34</v>
       </c>
       <c r="G3" t="s" s="6">
@@ -1751,7 +1757,7 @@
       <c r="H3" t="s" s="6">
         <v>35</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="14">
         <v>91.875</v>
       </c>
       <c r="J3" s="9">
@@ -1797,7 +1803,7 @@
       <c r="E4" t="s" s="8">
         <v>40</v>
       </c>
-      <c r="F4" t="s" s="10">
+      <c r="F4" t="s" s="13">
         <v>41</v>
       </c>
       <c r="G4" t="s" s="6">
@@ -1806,7 +1812,7 @@
       <c r="H4" t="s" s="6">
         <v>42</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="14">
         <v>65.625</v>
       </c>
       <c r="J4" s="9">
@@ -1852,7 +1858,7 @@
       <c r="E5" t="s" s="8">
         <v>46</v>
       </c>
-      <c r="F5" t="s" s="10">
+      <c r="F5" t="s" s="13">
         <v>47</v>
       </c>
       <c r="G5" t="s" s="6">
@@ -1861,7 +1867,7 @@
       <c r="H5" t="s" s="6">
         <v>48</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="14">
         <v>65.625</v>
       </c>
       <c r="J5" s="9">
@@ -1907,7 +1913,7 @@
       <c r="E6" t="s" s="8">
         <v>52</v>
       </c>
-      <c r="F6" t="s" s="10">
+      <c r="F6" t="s" s="13">
         <v>53</v>
       </c>
       <c r="G6" t="s" s="6">
@@ -1916,7 +1922,7 @@
       <c r="H6" t="s" s="6">
         <v>54</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="14">
         <v>46.875</v>
       </c>
       <c r="J6" s="9">
@@ -1934,7 +1940,7 @@
       <c r="N6" t="s" s="6">
         <v>23</v>
       </c>
-      <c r="O6" t="s" s="6">
+      <c r="O6" t="s" s="10">
         <v>55</v>
       </c>
       <c r="P6" s="11"/>
@@ -1962,7 +1968,7 @@
       <c r="E7" t="s" s="8">
         <v>58</v>
       </c>
-      <c r="F7" t="s" s="10">
+      <c r="F7" t="s" s="13">
         <v>59</v>
       </c>
       <c r="G7" t="s" s="6">
@@ -1971,7 +1977,7 @@
       <c r="H7" t="s" s="6">
         <v>60</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="14">
         <v>56.25</v>
       </c>
       <c r="J7" s="9">
@@ -2017,7 +2023,7 @@
       <c r="E8" t="s" s="8">
         <v>65</v>
       </c>
-      <c r="F8" t="s" s="10">
+      <c r="F8" t="s" s="13">
         <v>66</v>
       </c>
       <c r="G8" t="s" s="6">
@@ -2026,7 +2032,7 @@
       <c r="H8" t="s" s="6">
         <v>67</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="14">
         <v>106.875</v>
       </c>
       <c r="J8" s="9">
@@ -2072,7 +2078,7 @@
       <c r="E9" t="s" s="8">
         <v>71</v>
       </c>
-      <c r="F9" t="s" s="10">
+      <c r="F9" t="s" s="13">
         <v>72</v>
       </c>
       <c r="G9" t="s" s="6">
@@ -2081,7 +2087,7 @@
       <c r="H9" t="s" s="6">
         <v>73</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="14">
         <v>10.875</v>
       </c>
       <c r="J9" s="9">
@@ -2125,7 +2131,7 @@
       <c r="E10" t="s" s="8">
         <v>77</v>
       </c>
-      <c r="F10" t="s" s="10">
+      <c r="F10" t="s" s="13">
         <v>78</v>
       </c>
       <c r="G10" t="s" s="6">
@@ -2134,7 +2140,7 @@
       <c r="H10" t="s" s="6">
         <v>79</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="14">
         <v>71.25</v>
       </c>
       <c r="J10" s="9">
@@ -2167,59 +2173,59 @@
       <c r="W10" s="12"/>
     </row>
     <row r="11" ht="19.9" customHeight="1">
-      <c r="A11" t="s" s="14">
+      <c r="A11" t="s" s="15">
         <v>80</v>
       </c>
-      <c r="B11" t="s" s="15">
+      <c r="B11" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="C11" t="s" s="15">
+      <c r="C11" t="s" s="16">
         <v>81</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" t="s" s="17">
+      <c r="D11" s="17"/>
+      <c r="E11" t="s" s="18">
         <v>82</v>
       </c>
-      <c r="F11" t="s" s="18">
+      <c r="F11" t="s" s="19">
         <v>83</v>
       </c>
-      <c r="G11" t="s" s="15">
+      <c r="G11" t="s" s="16">
         <v>27</v>
       </c>
-      <c r="H11" t="s" s="15">
+      <c r="H11" t="s" s="16">
         <v>84</v>
       </c>
-      <c r="I11" s="19">
+      <c r="I11" s="20">
         <v>91.875</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="21">
         <v>1000</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="21">
         <v>25</v>
       </c>
-      <c r="L11" t="s" s="15">
+      <c r="L11" t="s" s="16">
         <v>80</v>
       </c>
-      <c r="M11" t="s" s="17">
+      <c r="M11" t="s" s="18">
         <v>82</v>
       </c>
-      <c r="N11" t="s" s="15">
+      <c r="N11" t="s" s="16">
         <v>23</v>
       </c>
-      <c r="O11" t="s" s="18">
+      <c r="O11" t="s" s="22">
         <v>36</v>
       </c>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="21"/>
-      <c r="S11" s="16"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="16"/>
-      <c r="V11" t="s" s="15">
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="23"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="17"/>
+      <c r="V11" t="s" s="16">
         <v>85</v>
       </c>
-      <c r="W11" s="22"/>
+      <c r="W11" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>